<commit_message>
Fixed single digit yards problem
</commit_message>
<xml_diff>
--- a/Data/Game_400876570_CLEM_ALA_.xlsx
+++ b/Data/Game_400876570_CLEM_ALA_.xlsx
@@ -1055,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1207,7 +1207,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>183</v>
@@ -1267,7 +1267,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>58</v>
@@ -1327,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>177</v>
@@ -1387,7 +1387,7 @@
         <v>9</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>236</v>
@@ -1567,7 +1567,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>241</v>
@@ -1627,7 +1627,7 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="E10">
         <v>84</v>
@@ -1728,7 +1728,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -1769,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="E13">
         <v>93</v>
@@ -1810,7 +1810,7 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>105</v>
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>116</v>
@@ -1933,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>45</v>
@@ -2097,7 +2097,7 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <v>191</v>
@@ -2179,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="E23">
         <v>63</v>
@@ -2261,7 +2261,7 @@
         <v>5</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E25">
         <v>186</v>
@@ -2302,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="E26">
         <v>61</v>
@@ -2343,7 +2343,7 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="E27">
         <v>173</v>
@@ -2384,7 +2384,7 @@
         <v>4</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E28">
         <v>106</v>
@@ -2507,7 +2507,7 @@
         <v>6</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <v>84</v>
@@ -2589,7 +2589,7 @@
         <v>6</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E33">
         <v>115</v>
@@ -2630,7 +2630,7 @@
         <v>6</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E34">
         <v>151</v>
@@ -2671,7 +2671,7 @@
         <v>9</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E35">
         <v>126</v>

</xml_diff>